<commit_message>
add destination and tests
</commit_message>
<xml_diff>
--- a/JavaBooks.xlsx
+++ b/JavaBooks.xlsx
@@ -35,7 +35,7 @@
     <t>PS123</t>
   </si>
   <si>
-    <t>июл 5 2017</t>
+    <t>июл 11 2017</t>
   </si>
   <si>
     <t>Kiev</t>
@@ -104,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B1:H3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -131,6 +131,9 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -151,6 +154,9 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>

</xml_diff>